<commit_message>
Avance en el programa principal
</commit_message>
<xml_diff>
--- a/Menu y Mensajes.xlsx
+++ b/Menu y Mensajes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="2" r:id="rId1"/>
@@ -5763,7 +5763,7 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5774,22 +5774,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="M56" sqref="M56"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="R59" sqref="R59:S60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16" width="2.140625" style="1" customWidth="1"/>
+    <col min="1" max="16" width="2.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R1" s="8" t="s">
         <v>24</v>
       </c>
       <c r="S1" s="8"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -5827,7 +5827,7 @@
       </c>
       <c r="S2" s="8"/>
     </row>
-    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -5847,11 +5847,11 @@
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
     </row>
-    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="S5" s="8"/>
     </row>
-    <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
@@ -5925,11 +5925,11 @@
       <c r="R6" s="8"/>
       <c r="S6" s="8"/>
     </row>
-    <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R7" s="8"/>
       <c r="S7" s="8"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -5969,7 +5969,7 @@
       </c>
       <c r="S8" s="8"/>
     </row>
-    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -5989,11 +5989,11 @@
       <c r="R9" s="8"/>
       <c r="S9" s="8"/>
     </row>
-    <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R10" s="8"/>
       <c r="S10" s="8"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>3</v>
       </c>
@@ -6045,7 +6045,7 @@
       </c>
       <c r="S11" s="8"/>
     </row>
-    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -6065,11 +6065,11 @@
       <c r="R12" s="8"/>
       <c r="S12" s="8"/>
     </row>
-    <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R13" s="8"/>
       <c r="S13" s="8"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>4</v>
       </c>
@@ -6121,7 +6121,7 @@
       </c>
       <c r="S14" s="8"/>
     </row>
-    <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -6141,11 +6141,11 @@
       <c r="R15" s="8"/>
       <c r="S15" s="8"/>
     </row>
-    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R16" s="8"/>
       <c r="S16" s="8"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>1</v>
       </c>
@@ -6189,7 +6189,7 @@
       </c>
       <c r="S17" s="8"/>
     </row>
-    <row r="18" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>1</v>
       </c>
@@ -6241,11 +6241,11 @@
       <c r="R18" s="8"/>
       <c r="S18" s="8"/>
     </row>
-    <row r="19" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R19" s="8"/>
       <c r="S19" s="8"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>1</v>
       </c>
@@ -6285,7 +6285,7 @@
       </c>
       <c r="S20" s="8"/>
     </row>
-    <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>2</v>
       </c>
@@ -6337,11 +6337,11 @@
       <c r="R21" s="8"/>
       <c r="S21" s="8"/>
     </row>
-    <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R22" s="8"/>
       <c r="S22" s="8"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>1</v>
       </c>
@@ -6381,7 +6381,7 @@
       </c>
       <c r="S23" s="8"/>
     </row>
-    <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>3</v>
       </c>
@@ -6433,11 +6433,11 @@
       <c r="R24" s="8"/>
       <c r="S24" s="8"/>
     </row>
-    <row r="25" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R25" s="8"/>
       <c r="S25" s="8"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>2</v>
       </c>
@@ -6485,7 +6485,7 @@
       </c>
       <c r="S26" s="8"/>
     </row>
-    <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>1</v>
       </c>
@@ -6519,11 +6519,11 @@
       <c r="R27" s="8"/>
       <c r="S27" s="8"/>
     </row>
-    <row r="28" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R28" s="8"/>
       <c r="S28" s="8"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>2</v>
       </c>
@@ -6575,7 +6575,7 @@
       </c>
       <c r="S29" s="8"/>
     </row>
-    <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>1</v>
       </c>
@@ -6609,11 +6609,11 @@
       <c r="R30" s="8"/>
       <c r="S30" s="8"/>
     </row>
-    <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R31" s="8"/>
       <c r="S31" s="8"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>3</v>
       </c>
@@ -6657,7 +6657,7 @@
       </c>
       <c r="S32" s="8"/>
     </row>
-    <row r="33" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -6683,11 +6683,11 @@
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
     </row>
-    <row r="34" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>3</v>
       </c>
@@ -6727,7 +6727,7 @@
       </c>
       <c r="S35" s="8"/>
     </row>
-    <row r="36" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -6753,11 +6753,11 @@
       <c r="R36" s="8"/>
       <c r="S36" s="8"/>
     </row>
-    <row r="37" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R37" s="8"/>
       <c r="S37" s="8"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>3</v>
       </c>
@@ -6797,7 +6797,7 @@
       </c>
       <c r="S38" s="8"/>
     </row>
-    <row r="39" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -6825,11 +6825,11 @@
       <c r="R39" s="8"/>
       <c r="S39" s="8"/>
     </row>
-    <row r="40" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R40" s="8"/>
       <c r="S40" s="8"/>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>4</v>
       </c>
@@ -6869,7 +6869,7 @@
       </c>
       <c r="S41" s="8"/>
     </row>
-    <row r="42" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -6907,11 +6907,11 @@
       <c r="R42" s="8"/>
       <c r="S42" s="8"/>
     </row>
-    <row r="43" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R43" s="8"/>
       <c r="S43" s="8"/>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>4</v>
       </c>
@@ -6951,7 +6951,7 @@
       </c>
       <c r="S44" s="8"/>
     </row>
-    <row r="45" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -6985,11 +6985,11 @@
       <c r="R45" s="8"/>
       <c r="S45" s="8"/>
     </row>
-    <row r="46" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R46" s="8"/>
       <c r="S46" s="8"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>4</v>
       </c>
@@ -7029,7 +7029,7 @@
       </c>
       <c r="S47" s="8"/>
     </row>
-    <row r="48" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="5"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -7065,11 +7065,11 @@
       <c r="R48" s="8"/>
       <c r="S48" s="8"/>
     </row>
-    <row r="49" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R49" s="8"/>
       <c r="S49" s="8"/>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>4</v>
       </c>
@@ -7107,7 +7107,7 @@
       </c>
       <c r="S50" s="8"/>
     </row>
-    <row r="51" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -7143,11 +7143,11 @@
       <c r="R51" s="8"/>
       <c r="S51" s="8"/>
     </row>
-    <row r="52" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R52" s="8"/>
       <c r="S52" s="8"/>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>3</v>
       </c>
@@ -7197,11 +7197,11 @@
         <v>10</v>
       </c>
       <c r="R53" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="S53" s="8"/>
     </row>
-    <row r="54" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>1</v>
       </c>
@@ -7229,11 +7229,11 @@
       <c r="R54" s="8"/>
       <c r="S54" s="8"/>
     </row>
-    <row r="55" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R55" s="8"/>
       <c r="S55" s="8"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>3</v>
       </c>
@@ -7277,11 +7277,11 @@
       <c r="O56" s="3"/>
       <c r="P56" s="4"/>
       <c r="R56" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="S56" s="8"/>
     </row>
-    <row r="57" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>1</v>
       </c>
@@ -7309,11 +7309,11 @@
       <c r="R57" s="8"/>
       <c r="S57" s="8"/>
     </row>
-    <row r="58" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R58" s="8"/>
       <c r="S58" s="8"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>3</v>
       </c>
@@ -7365,7 +7365,7 @@
       </c>
       <c r="S59" s="8"/>
     </row>
-    <row r="60" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>7</v>
       </c>
@@ -7413,11 +7413,11 @@
       <c r="R60" s="8"/>
       <c r="S60" s="8"/>
     </row>
-    <row r="61" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R61" s="8"/>
       <c r="S61" s="8"/>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>3</v>
       </c>
@@ -7469,7 +7469,7 @@
       </c>
       <c r="S62" s="8"/>
     </row>
-    <row r="63" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
         <v>7</v>
       </c>
@@ -7513,11 +7513,11 @@
       <c r="R63" s="8"/>
       <c r="S63" s="8"/>
     </row>
-    <row r="64" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R64" s="8"/>
       <c r="S64" s="8"/>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>3</v>
       </c>
@@ -7569,7 +7569,7 @@
       </c>
       <c r="S65" s="8"/>
     </row>
-    <row r="66" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>1</v>
       </c>
@@ -7619,11 +7619,11 @@
       <c r="R66" s="8"/>
       <c r="S66" s="8"/>
     </row>
-    <row r="67" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R67" s="8"/>
       <c r="S67" s="8"/>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>3</v>
       </c>
@@ -7673,7 +7673,7 @@
       <c r="R68" s="8"/>
       <c r="S68" s="8"/>
     </row>
-    <row r="69" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>8</v>
       </c>
@@ -7723,11 +7723,11 @@
       <c r="R69" s="8"/>
       <c r="S69" s="8"/>
     </row>
-    <row r="70" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R70" s="8"/>
       <c r="S70" s="8"/>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>3</v>
       </c>
@@ -7777,7 +7777,7 @@
       <c r="R71" s="8"/>
       <c r="S71" s="8"/>
     </row>
-    <row r="72" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
         <v>8</v>
       </c>
@@ -7825,11 +7825,11 @@
       <c r="R72" s="8"/>
       <c r="S72" s="8"/>
     </row>
-    <row r="73" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R73" s="8"/>
       <c r="S73" s="8"/>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>7</v>
       </c>
@@ -7877,7 +7877,7 @@
       </c>
       <c r="S74" s="8"/>
     </row>
-    <row r="75" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
         <v>7</v>
       </c>
@@ -7925,11 +7925,11 @@
       <c r="R75" s="8"/>
       <c r="S75" s="8"/>
     </row>
-    <row r="76" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R76" s="8"/>
       <c r="S76" s="8"/>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>3</v>
       </c>
@@ -7981,7 +7981,7 @@
       </c>
       <c r="S77" s="8"/>
     </row>
-    <row r="78" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="5"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
@@ -8017,11 +8017,11 @@
       <c r="R78" s="8"/>
       <c r="S78" s="8"/>
     </row>
-    <row r="79" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R79" s="8"/>
       <c r="S79" s="8"/>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -8041,7 +8041,7 @@
       <c r="R80" s="8"/>
       <c r="S80" s="8"/>
     </row>
-    <row r="81" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="5"/>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
@@ -8061,110 +8061,77 @@
       <c r="R81" s="8"/>
       <c r="S81" s="8"/>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
       <c r="R82" s="8"/>
       <c r="S82" s="8"/>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
       <c r="R83" s="8"/>
       <c r="S83" s="8"/>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
       <c r="R84" s="8"/>
       <c r="S84" s="8"/>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
       <c r="R85" s="8"/>
       <c r="S85" s="8"/>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="R86" s="8"/>
       <c r="S86" s="8"/>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
       <c r="R87" s="8"/>
       <c r="S87" s="8"/>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
       <c r="R88" s="8"/>
       <c r="S88" s="8"/>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
       <c r="R89" s="8"/>
       <c r="S89" s="8"/>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
       <c r="R90" s="8"/>
       <c r="S90" s="8"/>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
       <c r="R91" s="8"/>
       <c r="S91" s="8"/>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
       <c r="R92" s="8"/>
       <c r="S92" s="8"/>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
       <c r="R93" s="8"/>
       <c r="S93" s="8"/>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
       <c r="R94" s="8"/>
       <c r="S94" s="8"/>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
       <c r="R95" s="8"/>
       <c r="S95" s="8"/>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
       <c r="R96" s="8"/>
       <c r="S96" s="8"/>
     </row>
-    <row r="97" spans="18:19" x14ac:dyDescent="0.25">
+    <row r="97" spans="18:19" x14ac:dyDescent="0.3">
       <c r="R97" s="8"/>
       <c r="S97" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="R25:S25"/>
-    <mergeCell ref="R28:S28"/>
-    <mergeCell ref="R26:S27"/>
-    <mergeCell ref="R29:S30"/>
-    <mergeCell ref="R19:S19"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="R23:S24"/>
-    <mergeCell ref="R37:S37"/>
-    <mergeCell ref="R40:S40"/>
-    <mergeCell ref="R38:S39"/>
-    <mergeCell ref="R41:S42"/>
-    <mergeCell ref="R31:S31"/>
-    <mergeCell ref="R34:S34"/>
-    <mergeCell ref="R32:S33"/>
-    <mergeCell ref="R35:S36"/>
-    <mergeCell ref="R49:S49"/>
-    <mergeCell ref="R52:S52"/>
-    <mergeCell ref="R50:S51"/>
-    <mergeCell ref="R53:S54"/>
-    <mergeCell ref="R43:S43"/>
-    <mergeCell ref="R46:S46"/>
-    <mergeCell ref="R44:S45"/>
-    <mergeCell ref="R47:S48"/>
-    <mergeCell ref="R65:S66"/>
-    <mergeCell ref="R55:S55"/>
-    <mergeCell ref="R58:S58"/>
-    <mergeCell ref="R56:S57"/>
-    <mergeCell ref="R59:S60"/>
-    <mergeCell ref="R89:S90"/>
-    <mergeCell ref="R79:S79"/>
-    <mergeCell ref="R82:S82"/>
-    <mergeCell ref="R80:S81"/>
-    <mergeCell ref="R83:S84"/>
+    <mergeCell ref="R92:S93"/>
+    <mergeCell ref="R94:S94"/>
+    <mergeCell ref="R95:S96"/>
+    <mergeCell ref="R97:S97"/>
+    <mergeCell ref="R91:S91"/>
     <mergeCell ref="R17:S18"/>
     <mergeCell ref="R20:S21"/>
     <mergeCell ref="R85:S85"/>
@@ -8181,17 +8148,50 @@
     <mergeCell ref="R61:S61"/>
     <mergeCell ref="R64:S64"/>
     <mergeCell ref="R62:S63"/>
+    <mergeCell ref="R89:S90"/>
+    <mergeCell ref="R79:S79"/>
+    <mergeCell ref="R82:S82"/>
+    <mergeCell ref="R80:S81"/>
+    <mergeCell ref="R83:S84"/>
+    <mergeCell ref="R65:S66"/>
+    <mergeCell ref="R55:S55"/>
+    <mergeCell ref="R58:S58"/>
+    <mergeCell ref="R56:S57"/>
+    <mergeCell ref="R59:S60"/>
+    <mergeCell ref="R49:S49"/>
+    <mergeCell ref="R52:S52"/>
+    <mergeCell ref="R50:S51"/>
+    <mergeCell ref="R53:S54"/>
+    <mergeCell ref="R43:S43"/>
+    <mergeCell ref="R46:S46"/>
+    <mergeCell ref="R44:S45"/>
+    <mergeCell ref="R47:S48"/>
+    <mergeCell ref="R37:S37"/>
+    <mergeCell ref="R40:S40"/>
+    <mergeCell ref="R38:S39"/>
+    <mergeCell ref="R41:S42"/>
+    <mergeCell ref="R31:S31"/>
+    <mergeCell ref="R34:S34"/>
+    <mergeCell ref="R32:S33"/>
+    <mergeCell ref="R35:S36"/>
+    <mergeCell ref="R25:S25"/>
+    <mergeCell ref="R28:S28"/>
+    <mergeCell ref="R26:S27"/>
+    <mergeCell ref="R29:S30"/>
+    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="R23:S24"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="R4:S4"/>
     <mergeCell ref="R2:S3"/>
     <mergeCell ref="R5:S6"/>
     <mergeCell ref="R8:S9"/>
     <mergeCell ref="R11:S12"/>
     <mergeCell ref="R14:S15"/>
     <mergeCell ref="R13:S13"/>
-    <mergeCell ref="R92:S93"/>
-    <mergeCell ref="R94:S94"/>
-    <mergeCell ref="R95:S96"/>
-    <mergeCell ref="R97:S97"/>
-    <mergeCell ref="R91:S91"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Lectura y guardado en memoria FLASH
La flash tiene bastantes inconvenientes, pero bueno, es no volatil.
La idea es que cuando se escriba, escribir todo el mapa de memoria que defini, porque sino hay problemas con los bits que no se escriben. No hay que abusar de esta funcion ya que el numero de escrituras es limitado. Tener en cuenta para la logica. BESITO
</commit_message>
<xml_diff>
--- a/Menu y Mensajes.xlsx
+++ b/Menu y Mensajes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="50">
   <si>
     <t>I</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>Menu_4xc</t>
+  </si>
+  <si>
+    <t>K</t>
   </si>
 </sst>
 </file>
@@ -5774,8 +5777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="R59" sqref="R59:S60"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="Q82" sqref="Q82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8022,36 +8025,82 @@
       <c r="S79" s="8"/>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A80" s="2"/>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
-      <c r="G80" s="3"/>
+      <c r="A80" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="H80" s="3"/>
-      <c r="I80" s="3"/>
-      <c r="J80" s="3"/>
-      <c r="K80" s="3"/>
-      <c r="L80" s="3"/>
-      <c r="M80" s="3"/>
-      <c r="N80" s="3"/>
-      <c r="O80" s="3"/>
-      <c r="P80" s="4"/>
+      <c r="I80" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J80" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K80" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L80" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M80" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N80" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O80" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="P80" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="R80" s="8"/>
       <c r="S80" s="8"/>
     </row>
     <row r="81" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="5"/>
-      <c r="B81" s="6"/>
+      <c r="A81" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="C81" s="6"/>
       <c r="D81" s="6"/>
-      <c r="E81" s="6"/>
-      <c r="F81" s="6"/>
-      <c r="G81" s="6"/>
-      <c r="H81" s="6"/>
-      <c r="I81" s="6"/>
-      <c r="J81" s="6"/>
+      <c r="E81" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H81" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I81" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J81" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="K81" s="6"/>
       <c r="L81" s="6"/>
       <c r="M81" s="6"/>
@@ -8061,63 +8110,223 @@
       <c r="R81" s="8"/>
       <c r="S81" s="8"/>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R82" s="8"/>
       <c r="S82" s="8"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A83" s="2"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="3"/>
+      <c r="J83" s="3"/>
+      <c r="K83" s="3"/>
+      <c r="L83" s="3"/>
+      <c r="M83" s="3"/>
+      <c r="N83" s="3"/>
+      <c r="O83" s="3"/>
+      <c r="P83" s="4"/>
       <c r="R83" s="8"/>
       <c r="S83" s="8"/>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="5"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
+      <c r="J84" s="6"/>
+      <c r="K84" s="6"/>
+      <c r="L84" s="6"/>
+      <c r="M84" s="6"/>
+      <c r="N84" s="6"/>
+      <c r="O84" s="6"/>
+      <c r="P84" s="7"/>
       <c r="R84" s="8"/>
       <c r="S84" s="8"/>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R85" s="8"/>
       <c r="S85" s="8"/>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A86" s="2"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="3"/>
+      <c r="H86" s="3"/>
+      <c r="I86" s="3"/>
+      <c r="J86" s="3"/>
+      <c r="K86" s="3"/>
+      <c r="L86" s="3"/>
+      <c r="M86" s="3"/>
+      <c r="N86" s="3"/>
+      <c r="O86" s="3"/>
+      <c r="P86" s="4"/>
       <c r="R86" s="8"/>
       <c r="S86" s="8"/>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="5"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
+      <c r="J87" s="6"/>
+      <c r="K87" s="6"/>
+      <c r="L87" s="6"/>
+      <c r="M87" s="6"/>
+      <c r="N87" s="6"/>
+      <c r="O87" s="6"/>
+      <c r="P87" s="7"/>
       <c r="R87" s="8"/>
       <c r="S87" s="8"/>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R88" s="8"/>
       <c r="S88" s="8"/>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A89" s="2"/>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+      <c r="G89" s="3"/>
+      <c r="H89" s="3"/>
+      <c r="I89" s="3"/>
+      <c r="J89" s="3"/>
+      <c r="K89" s="3"/>
+      <c r="L89" s="3"/>
+      <c r="M89" s="3"/>
+      <c r="N89" s="3"/>
+      <c r="O89" s="3"/>
+      <c r="P89" s="4"/>
       <c r="R89" s="8"/>
       <c r="S89" s="8"/>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="5"/>
+      <c r="B90" s="6"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="6"/>
+      <c r="J90" s="6"/>
+      <c r="K90" s="6"/>
+      <c r="L90" s="6"/>
+      <c r="M90" s="6"/>
+      <c r="N90" s="6"/>
+      <c r="O90" s="6"/>
+      <c r="P90" s="7"/>
       <c r="R90" s="8"/>
       <c r="S90" s="8"/>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R91" s="8"/>
       <c r="S91" s="8"/>
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A92" s="2"/>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3"/>
+      <c r="G92" s="3"/>
+      <c r="H92" s="3"/>
+      <c r="I92" s="3"/>
+      <c r="J92" s="3"/>
+      <c r="K92" s="3"/>
+      <c r="L92" s="3"/>
+      <c r="M92" s="3"/>
+      <c r="N92" s="3"/>
+      <c r="O92" s="3"/>
+      <c r="P92" s="4"/>
       <c r="R92" s="8"/>
       <c r="S92" s="8"/>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="5"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="6"/>
+      <c r="J93" s="6"/>
+      <c r="K93" s="6"/>
+      <c r="L93" s="6"/>
+      <c r="M93" s="6"/>
+      <c r="N93" s="6"/>
+      <c r="O93" s="6"/>
+      <c r="P93" s="7"/>
       <c r="R93" s="8"/>
       <c r="S93" s="8"/>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R94" s="8"/>
       <c r="S94" s="8"/>
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A95" s="2"/>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="3"/>
+      <c r="H95" s="3"/>
+      <c r="I95" s="3"/>
+      <c r="J95" s="3"/>
+      <c r="K95" s="3"/>
+      <c r="L95" s="3"/>
+      <c r="M95" s="3"/>
+      <c r="N95" s="3"/>
+      <c r="O95" s="3"/>
+      <c r="P95" s="4"/>
       <c r="R95" s="8"/>
       <c r="S95" s="8"/>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="5"/>
+      <c r="B96" s="6"/>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="6"/>
+      <c r="J96" s="6"/>
+      <c r="K96" s="6"/>
+      <c r="L96" s="6"/>
+      <c r="M96" s="6"/>
+      <c r="N96" s="6"/>
+      <c r="O96" s="6"/>
+      <c r="P96" s="7"/>
       <c r="R96" s="8"/>
       <c r="S96" s="8"/>
     </row>
@@ -8127,11 +8336,50 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="R92:S93"/>
-    <mergeCell ref="R94:S94"/>
-    <mergeCell ref="R95:S96"/>
-    <mergeCell ref="R97:S97"/>
-    <mergeCell ref="R91:S91"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="R2:S3"/>
+    <mergeCell ref="R5:S6"/>
+    <mergeCell ref="R8:S9"/>
+    <mergeCell ref="R11:S12"/>
+    <mergeCell ref="R14:S15"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="R25:S25"/>
+    <mergeCell ref="R28:S28"/>
+    <mergeCell ref="R26:S27"/>
+    <mergeCell ref="R29:S30"/>
+    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="R23:S24"/>
+    <mergeCell ref="R37:S37"/>
+    <mergeCell ref="R40:S40"/>
+    <mergeCell ref="R38:S39"/>
+    <mergeCell ref="R41:S42"/>
+    <mergeCell ref="R31:S31"/>
+    <mergeCell ref="R34:S34"/>
+    <mergeCell ref="R32:S33"/>
+    <mergeCell ref="R35:S36"/>
+    <mergeCell ref="R49:S49"/>
+    <mergeCell ref="R52:S52"/>
+    <mergeCell ref="R50:S51"/>
+    <mergeCell ref="R53:S54"/>
+    <mergeCell ref="R43:S43"/>
+    <mergeCell ref="R46:S46"/>
+    <mergeCell ref="R44:S45"/>
+    <mergeCell ref="R47:S48"/>
+    <mergeCell ref="R65:S66"/>
+    <mergeCell ref="R55:S55"/>
+    <mergeCell ref="R58:S58"/>
+    <mergeCell ref="R56:S57"/>
+    <mergeCell ref="R59:S60"/>
+    <mergeCell ref="R89:S90"/>
+    <mergeCell ref="R79:S79"/>
+    <mergeCell ref="R82:S82"/>
+    <mergeCell ref="R80:S81"/>
+    <mergeCell ref="R83:S84"/>
     <mergeCell ref="R17:S18"/>
     <mergeCell ref="R20:S21"/>
     <mergeCell ref="R85:S85"/>
@@ -8148,50 +8396,11 @@
     <mergeCell ref="R61:S61"/>
     <mergeCell ref="R64:S64"/>
     <mergeCell ref="R62:S63"/>
-    <mergeCell ref="R89:S90"/>
-    <mergeCell ref="R79:S79"/>
-    <mergeCell ref="R82:S82"/>
-    <mergeCell ref="R80:S81"/>
-    <mergeCell ref="R83:S84"/>
-    <mergeCell ref="R65:S66"/>
-    <mergeCell ref="R55:S55"/>
-    <mergeCell ref="R58:S58"/>
-    <mergeCell ref="R56:S57"/>
-    <mergeCell ref="R59:S60"/>
-    <mergeCell ref="R49:S49"/>
-    <mergeCell ref="R52:S52"/>
-    <mergeCell ref="R50:S51"/>
-    <mergeCell ref="R53:S54"/>
-    <mergeCell ref="R43:S43"/>
-    <mergeCell ref="R46:S46"/>
-    <mergeCell ref="R44:S45"/>
-    <mergeCell ref="R47:S48"/>
-    <mergeCell ref="R37:S37"/>
-    <mergeCell ref="R40:S40"/>
-    <mergeCell ref="R38:S39"/>
-    <mergeCell ref="R41:S42"/>
-    <mergeCell ref="R31:S31"/>
-    <mergeCell ref="R34:S34"/>
-    <mergeCell ref="R32:S33"/>
-    <mergeCell ref="R35:S36"/>
-    <mergeCell ref="R25:S25"/>
-    <mergeCell ref="R28:S28"/>
-    <mergeCell ref="R26:S27"/>
-    <mergeCell ref="R29:S30"/>
-    <mergeCell ref="R19:S19"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="R23:S24"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="R2:S3"/>
-    <mergeCell ref="R5:S6"/>
-    <mergeCell ref="R8:S9"/>
-    <mergeCell ref="R11:S12"/>
-    <mergeCell ref="R14:S15"/>
-    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="R92:S93"/>
+    <mergeCell ref="R94:S94"/>
+    <mergeCell ref="R95:S96"/>
+    <mergeCell ref="R97:S97"/>
+    <mergeCell ref="R91:S91"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>